<commit_message>
Datenplatt_GIRA 24fach Schaltacktor hinzugefügt
</commit_message>
<xml_diff>
--- a/Elektro/Auflistung_KNX_Material.xlsx
+++ b/Elektro/Auflistung_KNX_Material.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Umbau\Elektro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente_Thomas_Brandl\GIT_Repository\Umbau\Elektro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C211CA73-9037-4891-9BFC-4009AE36C93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C709B1-F28D-4A8F-A233-8F8EF1DEFFB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{A6F8353D-0510-4489-8C99-156F73AB2641}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6F8353D-0510-4489-8C99-156F73AB2641}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -608,57 +608,6 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
     <dxf>
@@ -762,6 +711,57 @@
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9696"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -783,7 +783,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FFD03A8-96BD-4E09-BF02-3DEFE14EA902}" name="Tabelle1" displayName="Tabelle1" ref="A4:S20" totalsRowCount="1" headerRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3FFD03A8-96BD-4E09-BF02-3DEFE14EA902}" name="Tabelle1" displayName="Tabelle1" ref="A4:S20" totalsRowCount="1" headerRowDxfId="21">
   <autoFilter ref="A4:S19" xr:uid="{96AC54A7-3AF8-4232-A7CA-7456C1206A29}">
     <filterColumn colId="0">
       <filters>
@@ -808,29 +808,29 @@
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{F5042A58-498A-4C97-BACF-B3C8328DBC5F}" name="Bezeichnung"/>
     <tableColumn id="18" xr3:uid="{EBD698E9-BE7C-4EEA-BF83-B807A3FE3703}" name="Kanäle pro Gerät"/>
-    <tableColumn id="20" xr3:uid="{48770584-C7A0-4EFF-A5AB-7C1C84E8310E}" name="Kanäle gesamt" dataDxfId="26">
+    <tableColumn id="20" xr3:uid="{48770584-C7A0-4EFF-A5AB-7C1C84E8310E}" name="Kanäle gesamt" dataDxfId="20">
       <calculatedColumnFormula>Tabelle1[[#This Row],[Kanäle pro Gerät]]*Tabelle1[[#This Row],[Menge KNX-Geräte]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{FAF1D32A-393A-44C7-BE68-7B040F6D94CE}" name="TE"/>
-    <tableColumn id="19" xr3:uid="{D57E5FC7-9060-4F5D-BEF2-3E71373B4491}" name="Platzbedarf" dataDxfId="25">
+    <tableColumn id="19" xr3:uid="{D57E5FC7-9060-4F5D-BEF2-3E71373B4491}" name="Platzbedarf" dataDxfId="19">
       <calculatedColumnFormula>Tabelle1[[#This Row],[TE]]*SUM(Tabelle1[[#This Row],[Küche]:[Klo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{0CA81A17-BA15-4983-A8A2-0242A8B6B19B}" name="Herstellernummer" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{0CA81A17-BA15-4983-A8A2-0242A8B6B19B}" name="Herstellernummer" dataDxfId="18"/>
     <tableColumn id="4" xr3:uid="{4718EDFC-681A-42DA-B15F-DB810E8C969C}" name="Preis" dataCellStyle="Währung"/>
     <tableColumn id="5" xr3:uid="{A4E90C18-896F-4852-8F34-1136052F1D04}" name="Kategorie"/>
-    <tableColumn id="2" xr3:uid="{6085A278-C5F2-4B9B-81ED-75AC44992D6A}" name="Küche" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{71B99BB4-E121-4AC6-B2CC-B8283468FBBB}" name="Esszimmer" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{E4662B22-8FAD-414C-AAE6-B24E2CAB28D4}" name="Wohnzimmer" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{204170EB-6A51-4091-9F43-2BB5DD265154}" name="Speis" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{18FF780B-8CBB-488D-B52A-5E6374864CB2}" name="Bad" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{57EE2B1E-BB13-46B9-B6BC-CF4F5FCCDB66}" name="Gang" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{E92F9A3C-E1C5-4882-916E-DA389241E99B}" name="Schalafzimmer" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{3799BA4D-FAD2-475F-B312-0E659992795D}" name="Klo" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{6085A278-C5F2-4B9B-81ED-75AC44992D6A}" name="Küche" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{71B99BB4-E121-4AC6-B2CC-B8283468FBBB}" name="Esszimmer" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{E4662B22-8FAD-414C-AAE6-B24E2CAB28D4}" name="Wohnzimmer" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{204170EB-6A51-4091-9F43-2BB5DD265154}" name="Speis" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{18FF780B-8CBB-488D-B52A-5E6374864CB2}" name="Bad" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{57EE2B1E-BB13-46B9-B6BC-CF4F5FCCDB66}" name="Gang" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{E92F9A3C-E1C5-4882-916E-DA389241E99B}" name="Schalafzimmer" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{3799BA4D-FAD2-475F-B312-0E659992795D}" name="Klo" dataDxfId="10"/>
     <tableColumn id="17" xr3:uid="{17A122D9-4F1D-40D7-A3F8-16439D99B479}" name="KNX-fähig"/>
-    <tableColumn id="6" xr3:uid="{12170A0C-6A62-4A83-B4B9-2C3B5CC64F58}" name="Menge KNX-Geräte" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{12170A0C-6A62-4A83-B4B9-2C3B5CC64F58}" name="Menge KNX-Geräte" dataDxfId="9">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[KNX-fähig]]=1,SUM(Tabelle1[[#This Row],[Küche]:[Klo]]),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E30A86F8-AD60-4262-90C1-41270FEC02A0}" name="Endpreis" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6" dataCellStyle="Währung">
+    <tableColumn id="8" xr3:uid="{E30A86F8-AD60-4262-90C1-41270FEC02A0}" name="Endpreis" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0" dataCellStyle="Währung">
       <calculatedColumnFormula>SUM(Tabelle1[[#This Row],[Küche]:[Klo]])*Tabelle1[[#This Row],[Preis]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -839,7 +839,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AAEA202F-2E12-4951-852F-9E886146E92D}" name="Tabelle2" displayName="Tabelle2" ref="A2:K6" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AAEA202F-2E12-4951-852F-9E886146E92D}" name="Tabelle2" displayName="Tabelle2" ref="A2:K6" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A2:K6" xr:uid="{64997CFE-B058-4B80-8521-0376DB419888}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{A1D940C5-2DB8-4D38-B7EB-A7046EC82315}" name="Raum"/>
@@ -852,7 +852,7 @@
     <tableColumn id="8" xr3:uid="{523F6610-FD02-45F2-B727-E43C97AB7701}" name="Schalafzimmer"/>
     <tableColumn id="9" xr3:uid="{439EBBEB-C21F-4366-B359-B750404A6C1C}" name="Klo"/>
     <tableColumn id="11" xr3:uid="{21D0A73C-1259-4B5E-9160-E7893ABAD12E}" name="Hof"/>
-    <tableColumn id="10" xr3:uid="{3550BC49-49F6-41E8-A343-46EDD7312783}" name="Summe" dataDxfId="12">
+    <tableColumn id="10" xr3:uid="{3550BC49-49F6-41E8-A343-46EDD7312783}" name="Summe" dataDxfId="6">
       <calculatedColumnFormula>SUM(Tabelle2[[#This Row],[Küche]:[Hof]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -865,11 +865,11 @@
   <autoFilter ref="A1:F2" xr:uid="{2EE5AB28-B397-43CB-900D-A5B522ECDF9C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4DA6D9DF-2A14-4891-9CC3-08E42535F812}" name="Datum"/>
-    <tableColumn id="2" xr3:uid="{A2802040-74DD-489D-83C4-558D72967D5F}" name="Händler" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{5EE9FC28-C66B-4A96-9BA9-8280EC2E6589}" name="Kategorie" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{BD741B7D-FC24-407C-91C4-67731AA078DF}" name="Beschreibung" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{A87B7F3E-D2EF-4CAF-A80F-6E407E6EC1B1}" name="Konto" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{82BE7E6D-F523-4932-9103-8E1EB61BB46A}" name="Betrag" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{A2802040-74DD-489D-83C4-558D72967D5F}" name="Händler" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{5EE9FC28-C66B-4A96-9BA9-8280EC2E6589}" name="Kategorie" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{BD741B7D-FC24-407C-91C4-67731AA078DF}" name="Beschreibung" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A87B7F3E-D2EF-4CAF-A80F-6E407E6EC1B1}" name="Konto" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{82BE7E6D-F523-4932-9103-8E1EB61BB46A}" name="Betrag" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1193,27 +1193,27 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="3" width="6" customWidth="1" outlineLevel="2"/>
-    <col min="4" max="5" width="5.33203125" customWidth="1" outlineLevel="2"/>
-    <col min="6" max="6" width="71.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.28515625" customWidth="1" outlineLevel="2"/>
+    <col min="6" max="6" width="71.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="16" width="6" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1236,7 @@
       <c r="R1" s="24"/>
       <c r="S1" s="24"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1257,7 +1257,7 @@
       <c r="R2" s="24"/>
       <c r="S2" s="24"/>
     </row>
-    <row r="4" spans="1:19" s="3" customFormat="1" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" s="3" customFormat="1" ht="83.25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>216.84</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>51.16</v>
       </c>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>249.69</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>140.07</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>143.21</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>413.23</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>465.13</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>216.2</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>550.52</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>121.2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>237.51</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>131.35</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>336.17</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2066,13 +2066,13 @@
         <v>149.81</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S20" s="20">
         <f>SUBTOTAL(109,Tabelle1[Endpreis])</f>
         <v>3524.6899999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U21" s="12" t="s">
         <v>53</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U22" s="14" t="s">
         <v>54</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U23" s="12" t="s">
         <v>50</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U24" s="14" t="s">
         <v>51</v>
       </c>
@@ -2114,29 +2114,29 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="U21:V21">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="6" operator="between">
       <formula>21</formula>
       <formula>10000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThanOrEqual">
       <formula>$C$14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="greaterThan">
       <formula>$C$14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V24">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>$C$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="greaterThan">
       <formula>$C$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V21">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="lessThanOrEqual">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2168,19 +2168,19 @@
   <dimension ref="A2:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
     <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="73.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>55</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2315,20 +2315,20 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21">
         <v>44168</v>
       </c>
@@ -2380,18 +2380,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB6F161-F071-4988-9777-7297A2D0610F}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>79</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>80</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>81</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>82</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>100</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>85</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>86</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>87</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>82</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>101</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>102</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>89</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>85</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>90</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>91</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>94</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>92</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>82</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>100</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>96</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>97</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>98</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>99</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>82</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>100</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>82</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>125</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>

</xml_diff>